<commit_message>
EPBDS-8287 Remove dependency on BaseOpenlBuilderHelper
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/binding/ConditionalArrayIndexTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/binding/ConditionalArrayIndexTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>String</t>
   </si>
@@ -136,18 +136,6 @@
     <t>return arrayOfDrivers[select first having  numMovingViolations == 0];</t>
   </si>
   <si>
-    <t>Method Driver[] errorSelect(Driver[] arrayOfDrivers)</t>
-  </si>
-  <si>
-    <t>return arrayOfDrivers[@ age = 20];</t>
-  </si>
-  <si>
-    <t>Method Driver[] errorSelectLiteral(Driver[] arrayOfDrivers)</t>
-  </si>
-  <si>
-    <t>return arrayOfDrivers[select all having  numMovingViolations = 0];</t>
-  </si>
-  <si>
     <t>SelectStep</t>
   </si>
   <si>
@@ -169,12 +157,6 @@
     <t>=dd[!@ age &lt; $Age]</t>
   </si>
   <si>
-    <t>Spreadsheet Driver checkSpreadsheet1(Driver[] dd, int maxAge)</t>
-  </si>
-  <si>
-    <t>Spreadsheet Driver checkSpreadsheet2(Driver[] dd, int dIndex)</t>
-  </si>
-  <si>
     <t>Index:int</t>
   </si>
   <si>
@@ -182,6 +164,12 @@
   </si>
   <si>
     <t>=dd[!@ name == testDrivers[$Index].name]</t>
+  </si>
+  <si>
+    <t>Spreadsheet Driver checkSpreadsheet1(Driver[] dd, Integer maxAge)</t>
+  </si>
+  <si>
+    <t>Spreadsheet Driver checkSpreadsheet2(Driver[] dd, Integer dIndex)</t>
   </si>
 </sst>
 </file>
@@ -642,42 +630,42 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -981,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J30"/>
+  <dimension ref="B1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:I27"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,17 +989,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="F2" s="29" t="s">
+      <c r="C2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1221,141 +1209,117 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="F14" s="24" t="s">
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="F14" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="F15" s="21" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="F15" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="F17" s="24" t="s">
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="F17" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="F18" s="21" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="F18" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="G23" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="F21" s="24" t="s">
+      <c r="C25" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="26"/>
-    </row>
-    <row r="22" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="21" t="s">
+      <c r="G26" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-      <c r="F22" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="22"/>
-      <c r="H22" s="23"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="G27" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" t="s">
-        <v>48</v>
-      </c>
-      <c r="H28" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" t="s">
-        <v>44</v>
-      </c>
-      <c r="H29" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="I29" s="32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="G30" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>46</v>
+      <c r="H26" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="G27:I27"/>
+  <mergeCells count="12">
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="F14:H14"/>
@@ -1366,10 +1330,6 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="F22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>